<commit_message>
Schematic nearly done, ordened
</commit_message>
<xml_diff>
--- a/Connections.xlsx
+++ b/Connections.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7863ff1081637df6/Bureaublad/Sem6_Project/universal_connector_board/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D72E5123-5010-43D6-8209-8669714D33DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="8_{D72E5123-5010-43D6-8209-8669714D33DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DBC75013-EFC9-4F08-A395-6156D0C2B60F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DC364729-A95F-4A2A-BE67-225B29531981}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{DC364729-A95F-4A2A-BE67-225B29531981}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="72">
   <si>
     <t>GPIO</t>
   </si>
@@ -110,15 +110,6 @@
     <t>RX_PICO</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>INH</t>
-  </si>
-  <si>
     <t>Display1_CS</t>
   </si>
   <si>
@@ -168,6 +159,99 @@
   </si>
   <si>
     <t>MD1_EN</t>
+  </si>
+  <si>
+    <t>I/O Expander</t>
+  </si>
+  <si>
+    <t>STOP_PIN1</t>
+  </si>
+  <si>
+    <t>STOP_PIN2</t>
+  </si>
+  <si>
+    <t>MUX_A</t>
+  </si>
+  <si>
+    <t>MUX_B</t>
+  </si>
+  <si>
+    <t>MUX_INH</t>
+  </si>
+  <si>
+    <t>IOexp_INT</t>
+  </si>
+  <si>
+    <t>IOexp_SCL</t>
+  </si>
+  <si>
+    <t>IOexp_SDA</t>
+  </si>
+  <si>
+    <t>I2C SDA</t>
+  </si>
+  <si>
+    <t>I2C SCL</t>
+  </si>
+  <si>
+    <t>Radar_CS</t>
+  </si>
+  <si>
+    <t>Radar_RES</t>
+  </si>
+  <si>
+    <t>MD_SW1</t>
+  </si>
+  <si>
+    <t>MD_SW2</t>
+  </si>
+  <si>
+    <t>VCC</t>
+  </si>
+  <si>
+    <t>3.3V in</t>
+  </si>
+  <si>
+    <t>P0</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>SDA</t>
+  </si>
+  <si>
+    <t>SCL</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>P7</t>
+  </si>
+  <si>
+    <t>P6</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>P4</t>
   </si>
 </sst>
 </file>
@@ -289,8 +373,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -306,9 +393,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -321,9 +405,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -707,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9527733C-76B7-41C8-9E36-14F404F3D920}">
-  <dimension ref="C3:M24"/>
+  <dimension ref="C3:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -725,45 +808,45 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="2" t="s">
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
     </row>
     <row r="5" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
@@ -778,13 +861,13 @@
       <c r="F5" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="7"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="9"/>
       <c r="J5" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="K5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L5">
@@ -804,13 +887,13 @@
       <c r="F6" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="7"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="9"/>
       <c r="J6" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L6">
@@ -818,37 +901,37 @@
       </c>
     </row>
     <row r="7" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C7" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="12">
+      <c r="C7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2">
         <v>3</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="K7" s="13" t="s">
+      <c r="F7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="2">
         <v>38</v>
       </c>
-      <c r="M7" s="12" t="s">
+      <c r="M7" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="D8">
         <v>4</v>
@@ -859,13 +942,13 @@
       <c r="F8" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="7"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="9"/>
       <c r="J8" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="K8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L8">
@@ -874,7 +957,7 @@
     </row>
     <row r="9" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="D9">
         <v>5</v>
@@ -885,13 +968,13 @@
       <c r="F9" t="s">
         <v>0</v>
       </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="7"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="9"/>
       <c r="J9" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="11" t="s">
+      <c r="K9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L9">
@@ -911,13 +994,13 @@
       <c r="F10" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="7"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="9"/>
       <c r="J10" t="s">
         <v>19</v>
       </c>
-      <c r="K10" s="11" t="s">
+      <c r="K10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L10">
@@ -937,11 +1020,11 @@
       <c r="F11" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="7"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="9"/>
       <c r="J11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="K11">
         <v>28</v>
@@ -949,37 +1032,40 @@
       <c r="L11">
         <v>34</v>
       </c>
+      <c r="M11" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="12" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C12" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="12">
+      <c r="C12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2">
         <v>8</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="G12" s="5"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12">
+      <c r="F12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="8"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2">
         <v>33</v>
       </c>
-      <c r="M12" s="12" t="s">
+      <c r="M12" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="D13">
         <v>9</v>
@@ -990,11 +1076,11 @@
       <c r="F13" t="s">
         <v>0</v>
       </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="7"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="9"/>
       <c r="J13" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="K13">
         <v>27</v>
@@ -1002,10 +1088,13 @@
       <c r="L13">
         <v>32</v>
       </c>
+      <c r="M13" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="14" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="D14">
         <v>10</v>
@@ -1016,11 +1105,11 @@
       <c r="F14" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="7"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="9"/>
       <c r="J14" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="K14">
         <v>26</v>
@@ -1028,10 +1117,13 @@
       <c r="L14">
         <v>31</v>
       </c>
+      <c r="M14" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="15" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D15">
         <v>11</v>
@@ -1042,13 +1134,13 @@
       <c r="F15" t="s">
         <v>0</v>
       </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="11" t="s">
+      <c r="G15" s="8"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K15" s="11" t="s">
+      <c r="K15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L15">
@@ -1057,7 +1149,7 @@
     </row>
     <row r="16" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D16">
         <v>12</v>
@@ -1068,9 +1160,9 @@
       <c r="F16" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="5"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="7"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="9"/>
       <c r="K16">
         <v>22</v>
       </c>
@@ -1078,39 +1170,39 @@
         <v>29</v>
       </c>
       <c r="M16" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C17" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="12">
+      <c r="C17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2">
         <v>13</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="G17" s="5"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12">
+      <c r="F17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" s="8"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2">
         <v>28</v>
       </c>
-      <c r="M17" s="12" t="s">
+      <c r="M17" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D18">
         <v>14</v>
@@ -1119,11 +1211,11 @@
         <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>36</v>
-      </c>
-      <c r="G18" s="5"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="7"/>
+        <v>33</v>
+      </c>
+      <c r="G18" s="8"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="9"/>
       <c r="K18">
         <v>21</v>
       </c>
@@ -1131,12 +1223,12 @@
         <v>27</v>
       </c>
       <c r="M18" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D19">
         <v>15</v>
@@ -1145,11 +1237,11 @@
         <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>37</v>
-      </c>
-      <c r="G19" s="5"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="7"/>
+        <v>34</v>
+      </c>
+      <c r="G19" s="8"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="9"/>
       <c r="K19">
         <v>20</v>
       </c>
@@ -1157,12 +1249,12 @@
         <v>26</v>
       </c>
       <c r="M19" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D20">
         <v>16</v>
@@ -1173,9 +1265,9 @@
       <c r="F20" t="s">
         <v>10</v>
       </c>
-      <c r="G20" s="5"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="7"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="9"/>
       <c r="K20">
         <v>19</v>
       </c>
@@ -1183,12 +1275,12 @@
         <v>25</v>
       </c>
       <c r="M20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D21">
         <v>17</v>
@@ -1199,9 +1291,9 @@
       <c r="F21" t="s">
         <v>9</v>
       </c>
-      <c r="G21" s="5"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="7"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="9"/>
       <c r="K21">
         <v>18</v>
       </c>
@@ -1209,39 +1301,39 @@
         <v>24</v>
       </c>
       <c r="M21" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C22" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" s="12">
+      <c r="C22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2">
         <v>18</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F22" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="G22" s="5"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12">
+      <c r="F22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G22" s="8"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2">
         <v>23</v>
       </c>
-      <c r="M22" s="12" t="s">
+      <c r="M22" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="D23">
         <v>19</v>
@@ -1252,9 +1344,9 @@
       <c r="F23" t="s">
         <v>0</v>
       </c>
-      <c r="G23" s="5"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="7"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="9"/>
       <c r="K23">
         <v>17</v>
       </c>
@@ -1262,12 +1354,12 @@
         <v>22</v>
       </c>
       <c r="M23" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C24" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D24">
         <v>20</v>
@@ -1278,9 +1370,9 @@
       <c r="F24" t="s">
         <v>0</v>
       </c>
-      <c r="G24" s="8"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="12"/>
       <c r="K24">
         <v>16</v>
       </c>
@@ -1288,20 +1380,231 @@
         <v>21</v>
       </c>
       <c r="M24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C28" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="13"/>
+      <c r="E28" t="s">
+        <v>2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>4</v>
+      </c>
+      <c r="I28" t="s">
+        <v>4</v>
+      </c>
+      <c r="J28" t="s">
+        <v>2</v>
+      </c>
+      <c r="K28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C29" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" s="13"/>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29" t="s">
+        <v>62</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H29" s="4"/>
+      <c r="I29" t="s">
+        <v>56</v>
+      </c>
+      <c r="J29">
+        <v>16</v>
+      </c>
+      <c r="K29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C30" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="13"/>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30" t="s">
+        <v>63</v>
+      </c>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" t="s">
+        <v>65</v>
+      </c>
+      <c r="J30">
+        <v>15</v>
+      </c>
+      <c r="K30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C31" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="13"/>
+      <c r="E31">
+        <v>3</v>
+      </c>
+      <c r="F31" t="s">
+        <v>64</v>
+      </c>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" t="s">
+        <v>66</v>
+      </c>
+      <c r="J31">
+        <v>14</v>
+      </c>
+      <c r="K31" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C32" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" s="14"/>
+      <c r="E32">
+        <v>4</v>
+      </c>
+      <c r="F32" t="s">
+        <v>58</v>
+      </c>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" t="s">
+        <v>67</v>
+      </c>
+      <c r="J32">
+        <v>13</v>
+      </c>
+      <c r="K32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C33" s="14" t="s">
         <v>35</v>
       </c>
+      <c r="D33" s="14"/>
+      <c r="E33">
+        <v>5</v>
+      </c>
+      <c r="F33" t="s">
+        <v>59</v>
+      </c>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" t="s">
+        <v>68</v>
+      </c>
+      <c r="J33">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C34" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="14"/>
+      <c r="E34">
+        <v>6</v>
+      </c>
+      <c r="F34" t="s">
+        <v>60</v>
+      </c>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" t="s">
+        <v>69</v>
+      </c>
+      <c r="J34">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C35" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="14"/>
+      <c r="E35">
+        <v>7</v>
+      </c>
+      <c r="F35" t="s">
+        <v>61</v>
+      </c>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" t="s">
+        <v>70</v>
+      </c>
+      <c r="J35">
+        <v>10</v>
+      </c>
+      <c r="K35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C36" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" s="13"/>
+      <c r="E36">
+        <v>8</v>
+      </c>
+      <c r="F36" t="s">
+        <v>1</v>
+      </c>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" t="s">
+        <v>71</v>
+      </c>
+      <c r="J36">
+        <v>9</v>
+      </c>
+      <c r="K36" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="G4:I24"/>
+  <mergeCells count="19">
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="J3:J4"/>
+    <mergeCell ref="G29:H36"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="G4:I24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>